<commit_message>
fixes for multi-level categories.
</commit_message>
<xml_diff>
--- a/dexdata/data/dex-categories.xlsx
+++ b/dexdata/data/dex-categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\dexproducts\dexdata\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\digiseed\dex\dexproducts\dexdata\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA42D78-2FF3-4EB3-ABCE-07E4B842E503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F8ACBD-9668-41DD-94DE-6F2A708CAC52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EFDFF24D-C616-4E55-AA81-798350D91F4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EFDFF24D-C616-4E55-AA81-798350D91F4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Subcategories" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="266">
   <si>
     <t>slug</t>
   </si>
@@ -462,9 +462,6 @@
     <t>trade.jpg</t>
   </si>
   <si>
-    <t>Office</t>
-  </si>
-  <si>
     <t>Clips</t>
   </si>
   <si>
@@ -480,24 +477,12 @@
     <t>Correction Tape</t>
   </si>
   <si>
-    <t>Aprons and Caps</t>
-  </si>
-  <si>
-    <t>Aprons</t>
-  </si>
-  <si>
-    <t>Caps</t>
-  </si>
-  <si>
     <t>office</t>
   </si>
   <si>
     <t>office.jpg</t>
   </si>
   <si>
-    <t>aprons</t>
-  </si>
-  <si>
     <t>Corporate Gifts</t>
   </si>
   <si>
@@ -531,9 +516,6 @@
     <t>glue-tape</t>
   </si>
   <si>
-    <t>caps</t>
-  </si>
-  <si>
     <t>Cooling Towels</t>
   </si>
   <si>
@@ -838,6 +820,18 @@
   </si>
   <si>
     <t>os-bags</t>
+  </si>
+  <si>
+    <t>china-made-pens</t>
+  </si>
+  <si>
+    <t>klio-eterna-germany</t>
+  </si>
+  <si>
+    <t>maxema-italian</t>
+  </si>
+  <si>
+    <t>erga-italian</t>
   </si>
 </sst>
 </file>
@@ -1200,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{915DCBE6-D239-4E83-AEC1-3607E5ABAB39}">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,285 +1210,339 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" t="s">
         <v>189</v>
       </c>
-      <c r="C5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>187</v>
+        <v>262</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>199</v>
+        <v>263</v>
+      </c>
+      <c r="E15" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" t="s">
         <v>170</v>
-      </c>
-      <c r="B16" t="s">
-        <v>175</v>
-      </c>
-      <c r="C16" t="s">
-        <v>174</v>
-      </c>
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B17" t="s">
-        <v>176</v>
       </c>
       <c r="C17" t="s">
         <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="E17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18" t="s">
         <v>170</v>
       </c>
-      <c r="B18" t="s">
-        <v>176</v>
-      </c>
       <c r="C18" t="s">
-        <v>178</v>
-      </c>
-      <c r="D18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+      <c r="E19" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1505,7 +1553,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1516,7 +1564,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1527,7 +1575,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1538,18 +1586,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1560,7 +1608,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1571,7 +1619,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1582,7 +1630,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1593,18 +1641,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1615,7 +1663,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1631,7 +1679,7 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D33" t="s">
         <v>56</v>
@@ -1675,10 +1723,10 @@
         <v>29</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1705,7 +1753,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B40" t="s">
         <v>69</v>
@@ -1716,7 +1764,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B41" t="s">
         <v>70</v>
@@ -1727,7 +1775,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B42" t="s">
         <v>71</v>
@@ -1738,7 +1786,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B43" t="s">
         <v>72</v>
@@ -1749,7 +1797,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B44" t="s">
         <v>73</v>
@@ -1760,7 +1808,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B45" t="s">
         <v>74</v>
@@ -1771,7 +1819,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B46" t="s">
         <v>75</v>
@@ -1782,7 +1830,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B47" t="s">
         <v>76</v>
@@ -1862,10 +1910,10 @@
         <v>85</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1939,18 +1987,18 @@
         <v>101</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B62" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D62" t="s">
         <v>118</v>
@@ -1958,29 +2006,29 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D64" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B65" t="s">
         <v>116</v>
@@ -1992,81 +2040,81 @@
     </row>
     <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B72" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="D72" t="s">
         <v>127</v>
@@ -2074,10 +2122,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B73" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="D73" t="s">
         <v>128</v>
@@ -2085,7 +2133,7 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B74" t="s">
         <v>119</v>
@@ -2096,10 +2144,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B75" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="D75" t="s">
         <v>130</v>
@@ -2107,10 +2155,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B76" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D76" t="s">
         <v>131</v>
@@ -2118,10 +2166,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B77" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D77" t="s">
         <v>132</v>
@@ -2129,10 +2177,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B78" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D78" t="s">
         <v>133</v>
@@ -2140,7 +2188,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B79" t="s">
         <v>119</v>
@@ -2151,7 +2199,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B80" t="s">
         <v>120</v>
@@ -2165,7 +2213,7 @@
         <v>124</v>
       </c>
       <c r="B81" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D81" t="s">
         <v>136</v>
@@ -2176,10 +2224,10 @@
         <v>124</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="83" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2187,18 +2235,18 @@
         <v>124</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B84" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D84" t="s">
         <v>138</v>
@@ -2206,7 +2254,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B85" t="s">
         <v>137</v>
@@ -2217,343 +2265,321 @@
     </row>
     <row r="86" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>259</v>
+      </c>
+      <c r="B88" t="s">
         <v>142</v>
       </c>
-      <c r="B88" t="s">
+      <c r="D88" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B89" t="s">
         <v>143</v>
       </c>
-      <c r="D88" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>142</v>
-      </c>
-      <c r="B89" t="s">
+      <c r="D89" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B90" t="s">
         <v>144</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D90" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B91" t="s">
+        <v>239</v>
+      </c>
+      <c r="D91" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B92" t="s">
+        <v>240</v>
+      </c>
+      <c r="D92" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B93" t="s">
+        <v>145</v>
+      </c>
+      <c r="D93" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B94" t="s">
+        <v>146</v>
+      </c>
+      <c r="D94" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>142</v>
-      </c>
-      <c r="B90" t="s">
-        <v>145</v>
-      </c>
-      <c r="D90" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B95" t="s">
+        <v>241</v>
+      </c>
+      <c r="D95" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>142</v>
-      </c>
-      <c r="B91" t="s">
-        <v>245</v>
-      </c>
-      <c r="D91" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>142</v>
-      </c>
-      <c r="B92" t="s">
-        <v>246</v>
-      </c>
-      <c r="D92" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>142</v>
-      </c>
-      <c r="B93" t="s">
-        <v>146</v>
-      </c>
-      <c r="D93" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>142</v>
-      </c>
-      <c r="B94" t="s">
-        <v>147</v>
-      </c>
-      <c r="D94" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>142</v>
-      </c>
-      <c r="B95" t="s">
-        <v>247</v>
-      </c>
-      <c r="D95" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="96" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>142</v>
+        <v>259</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="97" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>142</v>
+        <v>259</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B98" t="s">
-        <v>149</v>
+        <v>73</v>
       </c>
       <c r="D98" t="s">
-        <v>153</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>148</v>
+        <v>196</v>
       </c>
       <c r="B99" t="s">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="D99" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>154</v>
+      <c r="A100" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="B100" t="s">
-        <v>73</v>
+        <v>201</v>
       </c>
       <c r="D100" t="s">
-        <v>81</v>
+        <v>215</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="A101" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B101" t="s">
         <v>202</v>
       </c>
-      <c r="B101" t="s">
-        <v>206</v>
-      </c>
       <c r="D101" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B102" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D102" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B103" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D103" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B104" t="s">
-        <v>209</v>
-      </c>
-      <c r="D104" t="s">
-        <v>218</v>
+        <v>205</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B105" t="s">
-        <v>210</v>
-      </c>
-      <c r="D105" t="s">
-        <v>222</v>
+        <v>206</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B106" t="s">
-        <v>211</v>
+        <v>101</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B107" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>202</v>
+      <c r="A108" t="s">
+        <v>167</v>
       </c>
       <c r="B108" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="B109" t="s">
+        <v>201</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D109" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>173</v>
-      </c>
       <c r="B110" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B111" t="s">
-        <v>207</v>
+        <v>101</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B112" t="s">
-        <v>85</v>
+        <v>210</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B113" t="s">
-        <v>101</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>225</v>
+        <v>164</v>
+      </c>
+      <c r="D113" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B114" t="s">
-        <v>216</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B115" t="s">
-        <v>170</v>
-      </c>
-      <c r="D115" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B116" t="s">
         <v>29</v>
       </c>
-      <c r="D116" t="s">
-        <v>267</v>
+      <c r="D114" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -2566,7 +2592,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2577,7 +2603,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2591,24 +2617,24 @@
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -2647,7 +2673,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B6" t="s">
         <v>66</v>
@@ -2689,7 +2715,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B9" t="s">
         <v>121</v>
@@ -2717,10 +2743,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B11" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C11" t="s">
         <v>140</v>
@@ -2731,72 +2757,72 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D12" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D13" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B14" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C14" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C15" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D15" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B16" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C16" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D16" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>